<commit_message>
added setup guide in readme file
</commit_message>
<xml_diff>
--- a/Functional and Non Functional testcases/api testcases.xlsx
+++ b/Functional and Non Functional testcases/api testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikra\OneDrive\Desktop\Exbanking\Exbanking\Functional and Non Functional testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65648213-0334-4E83-96C6-A4C853BF7F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4241A888-8D37-4C61-A751-346972CA431D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90AEBA1F-2E47-4930-8E78-CADE60AFD278}"/>
+    <workbookView xWindow="1860" yWindow="1260" windowWidth="21630" windowHeight="11310" xr2:uid="{90AEBA1F-2E47-4930-8E78-CADE60AFD278}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="498">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>TC_CREATE_USER_001</t>
-  </si>
-  <si>
     <t>Verify successful creation of a new user with valid input data</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>TC_CREATE_USER_002</t>
-  </si>
-  <si>
     <t>Verify error for creating a new user with already existing user data</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>json { "error": "Username already exists" }</t>
   </si>
   <si>
-    <t>TC_CREATE_USER_003</t>
-  </si>
-  <si>
     <t>Verify error for username with less than required characters</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>json { "error": "Username must be at least 3 characters long" }</t>
   </si>
   <si>
-    <t>TC_CREATE_USER_004</t>
-  </si>
-  <si>
     <t>Verify error for username with more than required characters</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
     <t>json { "error": "Username must be at most 20 characters long" }</t>
   </si>
   <si>
-    <t>TC_CREATE_USER_005</t>
-  </si>
-  <si>
     <t>Verify error for creating a user account with a negative balance</t>
   </si>
   <si>
@@ -135,12 +120,6 @@
     <t>create_user API test cases</t>
   </si>
   <si>
-    <t>json { "username": "vikram_with_an_extra_long_username", "password": "securePass123", "email": "vikram@test.com" } "balance": -100.00 }</t>
-  </si>
-  <si>
-    <t>TC_DEPOSIT_001</t>
-  </si>
-  <si>
     <t>Verify successful deposit</t>
   </si>
   <si>
@@ -150,57 +129,30 @@
     <t>User account with ID "12345" exists and is active.</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "amount": 100.00 }</t>
-  </si>
-  <si>
-    <t>json { "user_id": "12345", "new_balance": 100.00 }</t>
-  </si>
-  <si>
-    <t>TC_DEPOSIT_002</t>
-  </si>
-  <si>
     <t>Verify deposit with invalid user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to deposit funds to an invalid user ID.</t>
   </si>
   <si>
-    <t>json { "user_id": "99999", "amount": 100.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "User ID not found" }</t>
   </si>
   <si>
-    <t>TC_DEPOSIT_003</t>
-  </si>
-  <si>
     <t>Verify deposit with negative amount</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to deposit a negative amount.</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "amount": -50.00 }</t>
-  </si>
-  <si>
-    <t>TC_DEPOSIT_004</t>
-  </si>
-  <si>
     <t>Verify deposit with zero amount</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to deposit an amount of zero.</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "amount": 0.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Deposit amount must be greater than zero" }</t>
   </si>
   <si>
-    <t>TC_DEPOSIT_005</t>
-  </si>
-  <si>
     <t>Verify deposit when user account is inactive</t>
   </si>
   <si>
@@ -210,30 +162,18 @@
     <t>User account with ID "67890" exists and is inactive.</t>
   </si>
   <si>
-    <t>json { "user_id": "67890", "amount": 100.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "User account is inactive" }</t>
   </si>
   <si>
-    <t>TC_DEPOSIT_006</t>
-  </si>
-  <si>
     <t>Verify deposit without specifying user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when the user ID is not provided in the request.</t>
   </si>
   <si>
-    <t>json { "amount": 100.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "User ID is required" }</t>
   </si>
   <si>
-    <t>TC_DEPOSIT_007</t>
-  </si>
-  <si>
     <t>Verify deposit without specifying amount</t>
   </si>
   <si>
@@ -246,9 +186,6 @@
     <t>json { "error": "Deposit amount is required" }</t>
   </si>
   <si>
-    <t>TC_DEPOSIT_008</t>
-  </si>
-  <si>
     <t>Verify deposit with non-numeric amount</t>
   </si>
   <si>
@@ -261,66 +198,36 @@
     <t>json { "error": "Deposit amount must be a number" }</t>
   </si>
   <si>
-    <t>TC_DEPOSIT_009</t>
-  </si>
-  <si>
     <t>Verify deposit with large amount</t>
   </si>
   <si>
     <t>Ensure that the API can handle large deposit amounts without error.</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "amount": 1000000.00 }</t>
-  </si>
-  <si>
-    <t>json { "user_id": "12345", "new_balance": 1000000.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Deposit amount must be greater than 0" }</t>
   </si>
   <si>
-    <t>TC_WITHDRAW_001</t>
-  </si>
-  <si>
     <t>Verify successful withdrawal</t>
   </si>
   <si>
     <t>Ensure that funds are successfully withdrawn from the user's account if sufficient balance is available.</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "amount": 50.00 }</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_002</t>
-  </si>
-  <si>
     <t>Verify withdrawal with insufficient balance</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to withdraw more funds than available in the account.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists and has a balance of 50.00.</t>
-  </si>
-  <si>
     <t>json { "error": "Insufficient balance" }</t>
   </si>
   <si>
-    <t>TC_WITHDRAW_003</t>
-  </si>
-  <si>
     <t>Verify withdrawal with invalid user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to withdraw funds from an invalid user ID.</t>
   </si>
   <si>
-    <t>json { "user_id": "99999", "amount": 50.00 }</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_004</t>
-  </si>
-  <si>
     <t>Verify withdrawal with negative amount</t>
   </si>
   <si>
@@ -330,9 +237,6 @@
     <t>json { "error": "Withdrawal amount must be positive" }</t>
   </si>
   <si>
-    <t>TC_WITHDRAW_005</t>
-  </si>
-  <si>
     <t>Verify withdrawal with zero amount</t>
   </si>
   <si>
@@ -342,30 +246,15 @@
     <t>json { "error": "Withdrawal amount must be greater than zero" }</t>
   </si>
   <si>
-    <t>TC_WITHDRAW_006</t>
-  </si>
-  <si>
     <t>Verify withdrawal when user account is inactive</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to withdraw funds from an inactive user account.</t>
   </si>
   <si>
-    <t>json { "user_id": "67890", "amount": 50.00 }</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_007</t>
-  </si>
-  <si>
     <t>Verify withdrawal without specifying user ID</t>
   </si>
   <si>
-    <t>json { "amount": 50.00 }</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_008</t>
-  </si>
-  <si>
     <t>Verify withdrawal without specifying amount</t>
   </si>
   <si>
@@ -375,9 +264,6 @@
     <t>json { "error": "Withdrawal amount is required" }</t>
   </si>
   <si>
-    <t>TC_WITHDRAW_009</t>
-  </si>
-  <si>
     <t>Verify withdrawal with non-numeric amount</t>
   </si>
   <si>
@@ -390,30 +276,15 @@
     <t>json { "error": "Withdrawal amount must be a number" }</t>
   </si>
   <si>
-    <t>TC_WITHDRAW_010</t>
-  </si>
-  <si>
     <t>Ensure that the API can handle large withdrawal amounts without error.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists and has a balance of 1000000.00.</t>
-  </si>
-  <si>
-    <t>json { "user_id": "12345", "amount": 500000.00 }</t>
-  </si>
-  <si>
-    <t>User account with ID "12345" exists and has a balance of  150.00.</t>
-  </si>
-  <si>
     <t>Verify withdrawal with large amount above the withdrawal limit</t>
   </si>
   <si>
     <t>json { "message" : "Withdrawal amount must be lower than 50000" }</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_001</t>
-  </si>
-  <si>
     <t>Verify successful balance retrieval</t>
   </si>
   <si>
@@ -423,36 +294,21 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "balance": 100.00 }</t>
-  </si>
-  <si>
-    <t>TC_GET_BALANCE_002</t>
-  </si>
-  <si>
     <t>Verify balance retrieval with invalid user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to retrieve balance for an invalid user ID.</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_003</t>
-  </si>
-  <si>
     <t>Verify balance retrieval for inactive user account</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to retrieve balance for an inactive user account.</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_004</t>
-  </si>
-  <si>
     <t>Verify balance retrieval without specifying user ID</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_005</t>
-  </si>
-  <si>
     <t>Verify balance retrieval with special characters in user ID</t>
   </si>
   <si>
@@ -462,9 +318,6 @@
     <t>json { "error": "Invalid user ID format" }</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_006</t>
-  </si>
-  <si>
     <t>Verify balance retrieval with numeric user ID</t>
   </si>
   <si>
@@ -474,12 +327,6 @@
     <t>User account with ID "112233" exists and is active.</t>
   </si>
   <si>
-    <t>json { "user_id": "112233", "balance": 500.00 }</t>
-  </si>
-  <si>
-    <t>TC_GET_BALANCE_007</t>
-  </si>
-  <si>
     <t>Verify balance retrieval with alphanumeric user ID</t>
   </si>
   <si>
@@ -489,27 +336,12 @@
     <t>User account with ID "user123" exists and is active.</t>
   </si>
   <si>
-    <t>json { "user_id": "user123", "balance": 250.00 }</t>
-  </si>
-  <si>
-    <t>TC_GET_BALANCE_008</t>
-  </si>
-  <si>
     <t>Verify balance retrieval for user with high balance</t>
   </si>
   <si>
     <t>Ensure that the API can handle and accurately return a high balance amount.</t>
   </si>
   <si>
-    <t>User account with ID "45678" exists and has a high balance (e.g., 1,000,000.00).</t>
-  </si>
-  <si>
-    <t>json { "user_id": "45678", "balance": 1000000.00 }</t>
-  </si>
-  <si>
-    <t>TC_GET_BALANCE_009</t>
-  </si>
-  <si>
     <t>Verify balance retrieval for user with zero balance</t>
   </si>
   <si>
@@ -519,12 +351,6 @@
     <t>User account with ID "34567" exists and has a zero balance.</t>
   </si>
   <si>
-    <t>json { "user_id": "34567", "balance": 0.00 }</t>
-  </si>
-  <si>
-    <t>TC_GET_BALANCE_010</t>
-  </si>
-  <si>
     <t>Verify balance retrieval performance</t>
   </si>
   <si>
@@ -534,42 +360,18 @@
     <t>Response time is within acceptable limits (e.g., &lt;200ms).</t>
   </si>
   <si>
-    <t>TC_SEND_001</t>
-  </si>
-  <si>
     <t>Verify successful fund transfer</t>
   </si>
   <si>
     <t>Ensure that funds are successfully transferred from one user's account to another if sufficient balance is available.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists with a balance of 100.00. User account with ID "67890" exists.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 50.00 }</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "new_balance": 50.00, "to_user_id": "67890", "new_balance": 50.00 }</t>
-  </si>
-  <si>
-    <t>TC_SEND_002</t>
-  </si>
-  <si>
     <t>Verify transfer with insufficient balance</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to transfer more funds than available in the sender's account.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists with a balance of 50.00. User account with ID "67890" exists.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 100.00 }</t>
-  </si>
-  <si>
-    <t>TC_SEND_003</t>
-  </si>
-  <si>
     <t>Verify transfer with invalid sender user ID</t>
   </si>
   <si>
@@ -579,63 +381,36 @@
     <t>User account with ID "67890" exists.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "99999", "to_user_id": "67890", "amount": 50.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Sender user ID not found" }</t>
   </si>
   <si>
-    <t>TC_SEND_004</t>
-  </si>
-  <si>
     <t>Verify transfer with invalid recipient user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to transfer funds to an invalid recipient user ID.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists with a balance of 100.00.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "99999", "amount": 50.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Recipient user ID not found" }</t>
   </si>
   <si>
-    <t>TC_SEND_005</t>
-  </si>
-  <si>
     <t>Verify transfer with negative amount</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to transfer a negative amount.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": -50.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Transfer amount must be positive" }</t>
   </si>
   <si>
-    <t>TC_SEND_006</t>
-  </si>
-  <si>
     <t>Verify transfer with zero amount</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to transfer an amount of zero.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 0.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Transfer amount must be greater than zero" }</t>
   </si>
   <si>
-    <t>TC_SEND_007</t>
-  </si>
-  <si>
     <t>Verify transfer when sender user account is inactive</t>
   </si>
   <si>
@@ -648,57 +423,33 @@
     <t>json { "error": "Sender user account is inactive" }</t>
   </si>
   <si>
-    <t>TC_SEND_008</t>
-  </si>
-  <si>
     <t>Verify transfer when recipient user account is inactive</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to transfer funds to an inactive recipient user account.</t>
   </si>
   <si>
-    <t>Sender user account with ID "12345" exists with a balance of 100.00. Recipient user account with ID "67890" exists and is inactive.</t>
-  </si>
-  <si>
     <t>json { "error": "Recipient user account is inactive" }</t>
   </si>
   <si>
-    <t>TC_SEND_009</t>
-  </si>
-  <si>
     <t>Verify transfer without specifying sender user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when the sender user ID is not provided in the request.</t>
   </si>
   <si>
-    <t>json { "to_user_id": "67890", "amount": 50.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Sender user ID is required" }</t>
   </si>
   <si>
-    <t>TC_SEND_010</t>
-  </si>
-  <si>
     <t>Verify transfer without specifying recipient user ID</t>
   </si>
   <si>
     <t>Validate that the API returns an error when the recipient user ID is not provided in the request.</t>
   </si>
   <si>
-    <t>Sender user account with ID "12345" exists with a balance of 100.00.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "amount": 50.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Recipient user ID is required" }</t>
   </si>
   <si>
-    <t>TC_SEND_011</t>
-  </si>
-  <si>
     <t>Verify transfer without specifying amount</t>
   </si>
   <si>
@@ -708,114 +459,60 @@
     <t>User accounts with IDs "12345" and "67890" exist.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890" }</t>
-  </si>
-  <si>
     <t>json { "error": "Transfer amount is required" }</t>
   </si>
   <si>
-    <t>TC_SEND_012</t>
-  </si>
-  <si>
     <t>Verify transfer with non-numeric amount</t>
   </si>
   <si>
     <t>Validate that the API returns an error when the transfer amount is not a valid number.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": "fifty" }</t>
-  </si>
-  <si>
     <t>json { "error": "Transfer amount must be a number" }</t>
   </si>
   <si>
-    <t>TC_SEND_013</t>
-  </si>
-  <si>
     <t>Verify transfer with large amount</t>
   </si>
   <si>
     <t>Ensure that the API can handle large transfer amounts without error.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists with a balance of 1,000,000.00. User account with ID "67890" exists.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 500000.00 }</t>
-  </si>
-  <si>
-    <t>```json { "from_user_id": "12345", "new_balance": 500000.00,</t>
-  </si>
-  <si>
-    <t>TC_SEND_014</t>
-  </si>
-  <si>
     <t>Verify sending money to a deactivated user</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to send money to a deactivated user.</t>
   </si>
   <si>
-    <t>Sender user account with ID "12345" exists and is active with a balance of 100.00. Recipient user account with ID "67890" exists and is deactivated.</t>
-  </si>
-  <si>
     <t>json { "error": "Recipient user account is deactivated" }</t>
   </si>
   <si>
-    <t>TC_SEND_015</t>
-  </si>
-  <si>
     <t>Verify sending money to a user who has not completed verification</t>
   </si>
   <si>
     <t>Validate that the API returns an error when trying to send money to a user who has not completed verification.</t>
   </si>
   <si>
-    <t>Sender user account with ID "12345" exists and is active with a balance of 100.00. Recipient user account with ID "67891" exists and is unverified.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67891", "amount": 50.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Recipient user account is not verified" }</t>
   </si>
   <si>
-    <t>TC_SEND_016</t>
-  </si>
-  <si>
     <t>Verify sending money with an amount below the minimum allowed</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to send an amount below the minimum allowed.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 0.50 }</t>
-  </si>
-  <si>
     <t>json { "error": "Transfer amount is below the minimum allowed" }</t>
   </si>
   <si>
-    <t>TC_SEND_017</t>
-  </si>
-  <si>
     <t>Verify sending money with an amount above the maximum allowed</t>
   </si>
   <si>
     <t>Ensure that the API returns an error when trying to send an amount above the maximum allowed.</t>
   </si>
   <si>
-    <t>User accounts with IDs "12345" and "67890" exist and are active. Maximum transfer amount is 10,000.00.</t>
-  </si>
-  <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 20000.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Transfer amount exceeds the maximum allowed" }</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_011</t>
-  </si>
-  <si>
     <t>Verify checking balance for a temporarily deactivated user</t>
   </si>
   <si>
@@ -828,9 +525,6 @@
     <t>json { "error": "User account is temporarily deactivated" }</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_012</t>
-  </si>
-  <si>
     <t>Verify checking balance for a user who has not completed verification</t>
   </si>
   <si>
@@ -843,9 +537,6 @@
     <t>json { "error": "User account has not completed verification" }</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_013</t>
-  </si>
-  <si>
     <t>Verify checking balance for a locked account</t>
   </si>
   <si>
@@ -858,9 +549,6 @@
     <t>json { "error": "User account is locked" }</t>
   </si>
   <si>
-    <t>TC_GET_BALANCE_014</t>
-  </si>
-  <si>
     <t>Verify checking balance for a closed account</t>
   </si>
   <si>
@@ -879,12 +567,6 @@
     <t>Ensure that the API returns an error when trying to withdraw an amount below the minimum allowed.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists and has a balance of 100.00. Minimum withdrawal amount is 10.00.</t>
-  </si>
-  <si>
-    <t>json { "user_id": "12345", "amount": 5.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Withdrawal amount is below the minimum allowed" }</t>
   </si>
   <si>
@@ -894,12 +576,6 @@
     <t>Ensure that the API returns an error when trying to withdraw an amount above the maximum allowed.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists and has a balance of 100.00. Maximum withdrawal amount is 1000.00.</t>
-  </si>
-  <si>
-    <t>json { "user_id": "12345", "amount": 1500.00 }</t>
-  </si>
-  <si>
     <t>json { "error": "Withdrawal amount exceeds the maximum allowed" }</t>
   </si>
   <si>
@@ -909,21 +585,6 @@
     <t>Ensure that the user's balance is updated correctly after making multiple consecutive withdrawals.</t>
   </si>
   <si>
-    <t>User account with ID "12345" exists and has a balance of 100.00.</t>
-  </si>
-  <si>
-    <t>json { "user_id": "12345", "amount": 20.00 }</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_011</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_012</t>
-  </si>
-  <si>
-    <t>TC_WITHDRAW_013</t>
-  </si>
-  <si>
     <t>deposit API test cases</t>
   </si>
   <si>
@@ -966,9 +627,6 @@
     <t>Ensure that the API returns an error when trying to deposit funds with an invalid currency.</t>
   </si>
   <si>
-    <t>json { "user_id": "12345", "amount": 100.00, "currency": "INVALID" }</t>
-  </si>
-  <si>
     <t>json { "error": "Invalid currency" }</t>
   </si>
   <si>
@@ -981,9 +639,6 @@
     <t>User account with ID "67890" exists and has restricted access.</t>
   </si>
   <si>
-    <t>json { "user_id": "67890", "amount": 100.00, "currency": "USD" }</t>
-  </si>
-  <si>
     <t>json { "error": "Account has restricted access" }</t>
   </si>
   <si>
@@ -993,9 +648,6 @@
     <t>Ensure that the API returns an error when trying to make a withdrawal from an account with restricted access.</t>
   </si>
   <si>
-    <t>TC_SEND_018</t>
-  </si>
-  <si>
     <t>Verify sending money with invalid currency</t>
   </si>
   <si>
@@ -1005,12 +657,6 @@
     <t>Sender user account with ID "12345" exists and has sufficient balance. Recipient user account with ID "67890" exists.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 50.00, "currency": "INVALID" }</t>
-  </si>
-  <si>
-    <t>TC_SEND_019</t>
-  </si>
-  <si>
     <t>Verify sending money to an account with restricted access</t>
   </si>
   <si>
@@ -1020,9 +666,6 @@
     <t>Sender user account with ID "12345" exists and has sufficient balance. Recipient user account with ID "67890" exists and has restricted access.</t>
   </si>
   <si>
-    <t>json { "from_user_id": "12345", "to_user_id": "67890", "amount": 50.00, "currency": "USD" }</t>
-  </si>
-  <si>
     <t>json { "error": "Recipient account has restricted access" }</t>
   </si>
   <si>
@@ -1030,9 +673,6 @@
   </si>
   <si>
     <t>System is up and running.</t>
-  </si>
-  <si>
-    <t>NFTC-010</t>
   </si>
   <si>
     <r>
@@ -1051,9 +691,6 @@
     <t>The response time for each request should be under 1 second under normal load.</t>
   </si>
   <si>
-    <t>NFTC-011</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Availability During Peak Traffic for </t>
     </r>
@@ -1070,9 +707,6 @@
     <t>The API should remain available and responsive, with response times within acceptable limits (e.g., under 3 seconds) during peak traffic.</t>
   </si>
   <si>
-    <t>NFTC-012</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Soak Testing for </t>
     </r>
@@ -1087,9 +721,6 @@
   </si>
   <si>
     <t>The system should handle the constant load over 24 hours without performance degradation or failures, maintaining response times under 2 seconds.</t>
-  </si>
-  <si>
-    <t>NFTC-001</t>
   </si>
   <si>
     <r>
@@ -1131,9 +762,6 @@
     </r>
   </si>
   <si>
-    <t>NFTC-009</t>
-  </si>
-  <si>
     <t>Test the API's performance with a high number of concurrent requests.</t>
   </si>
   <si>
@@ -1144,9 +772,6 @@
   </si>
   <si>
     <t>Perform soak testing to ensure the API's long-term reliability under continuous load.</t>
-  </si>
-  <si>
-    <t>NFTC-013</t>
   </si>
   <si>
     <r>
@@ -1168,9 +793,6 @@
     <t>The system should handle the high number of concurrent requests without crashing, with response times under 2 seconds.</t>
   </si>
   <si>
-    <t>NFTC-014</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Response Time under Normal Load for </t>
     </r>
@@ -1184,9 +806,6 @@
     </r>
   </si>
   <si>
-    <t>NFTC-015</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Availability During Peak Traffic for </t>
     </r>
@@ -1203,9 +822,6 @@
     <t>The API should remain available and responsive, with response times within acceptable limits (e.g., under 2 seconds) during peak traffic.</t>
   </si>
   <si>
-    <t>NFTC-016</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">High Concurrent Requests for </t>
     </r>
@@ -1222,9 +838,6 @@
     <t>Multiple user accounts with sufficient balance.</t>
   </si>
   <si>
-    <t>NFTC-017</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Response Time under Normal Load for </t>
     </r>
@@ -1238,9 +851,6 @@
     </r>
   </si>
   <si>
-    <t>NFTC-018</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Availability During Peak Traffic for </t>
     </r>
@@ -1254,9 +864,6 @@
     </r>
   </si>
   <si>
-    <t>NFTC-019</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">High Concurrent Requests for </t>
     </r>
@@ -1273,9 +880,6 @@
     <t>Large number of user accounts (e.g., 1 million users).</t>
   </si>
   <si>
-    <t>NFTC-020</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Response Time under Normal Load for </t>
     </r>
@@ -1287,9 +891,6 @@
       </rPr>
       <t>get_balance</t>
     </r>
-  </si>
-  <si>
-    <t>NFTC-021</t>
   </si>
   <si>
     <r>
@@ -1482,9 +1083,6 @@
     <t xml:space="preserve"> Send a POST request to the /withdraw endpoint with an amount above the maximum allowed.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Send a POST request to the /withdraw endpoint with an amount of 20.00 multiple times with different amount</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Verify that the API responds with a success message and the updated balance.</t>
   </si>
   <si>
@@ -1641,9 +1239,6 @@
     <t>Send requests</t>
   </si>
   <si>
-    <t>NFTC-006</t>
-  </si>
-  <si>
     <t>Usability Testing for API Responses</t>
   </si>
   <si>
@@ -1657,9 +1252,6 @@
   </si>
   <si>
     <t>API responses should be clear, concise, and informative, providing necessary details like error messages, transaction IDs, and status codes.</t>
-  </si>
-  <si>
-    <t>NFTC-007</t>
   </si>
   <si>
     <r>
@@ -1687,9 +1279,6 @@
     <t>The withdraw functionality should operate reliably over an extended period without failures or data integrity issues.</t>
   </si>
   <si>
-    <t>NFTC-008</t>
-  </si>
-  <si>
     <t>Recovery Testing for All APIs</t>
   </si>
   <si>
@@ -1705,15 +1294,6 @@
     <t>The system should recover automatically or with minimal manual intervention, resuming normal operations within a defined acceptable time.</t>
   </si>
   <si>
-    <t>NFTC-003</t>
-  </si>
-  <si>
-    <t>NFTC-004</t>
-  </si>
-  <si>
-    <t>NFTC-005</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Use a load testing tool to simulate 1000 concurrent create_user requests and Monitor the response times and system resource usage.</t>
   </si>
   <si>
@@ -1724,6 +1304,441 @@
   </si>
   <si>
     <t xml:space="preserve"> Simulate a system failure (e.g., server crash, database failure) and Observe the system's recovery process and time taken to resume normal operations.</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_01</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_02</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_03</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_04</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_05</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_06</t>
+  </si>
+  <si>
+    <t>TC_CREATE_USER_07</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_01</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_02</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_03</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_04</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_05</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_06</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_07</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_08</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_09</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_10</t>
+  </si>
+  <si>
+    <t>TC_DEPOSIT_11</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_01</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_02</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_03</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_04</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_05</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_06</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_07</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_08</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_09</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_10</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_11</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_12</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_13</t>
+  </si>
+  <si>
+    <t>TC_WITHDRAW_14</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_01</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_02</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_03</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_04</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_05</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_06</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_07</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_08</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_09</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_10</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_11</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_12</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_13</t>
+  </si>
+  <si>
+    <t>TC_GET_BALANCE_14</t>
+  </si>
+  <si>
+    <t>TC_SEND_01</t>
+  </si>
+  <si>
+    <t>TC_SEND_02</t>
+  </si>
+  <si>
+    <t>TC_SEND_03</t>
+  </si>
+  <si>
+    <t>TC_SEND_04</t>
+  </si>
+  <si>
+    <t>TC_SEND_05</t>
+  </si>
+  <si>
+    <t>TC_SEND_06</t>
+  </si>
+  <si>
+    <t>TC_SEND_07</t>
+  </si>
+  <si>
+    <t>TC_SEND_08</t>
+  </si>
+  <si>
+    <t>TC_SEND_09</t>
+  </si>
+  <si>
+    <t>TC_SEND_10</t>
+  </si>
+  <si>
+    <t>TC_SEND_11</t>
+  </si>
+  <si>
+    <t>TC_SEND_12</t>
+  </si>
+  <si>
+    <t>TC_SEND_13</t>
+  </si>
+  <si>
+    <t>TC_SEND_14</t>
+  </si>
+  <si>
+    <t>TC_SEND_15</t>
+  </si>
+  <si>
+    <t>TC_SEND_16</t>
+  </si>
+  <si>
+    <t>TC_SEND_17</t>
+  </si>
+  <si>
+    <t>TC_SEND_18</t>
+  </si>
+  <si>
+    <t>TC_SEND_19</t>
+  </si>
+  <si>
+    <t>NFTC-01</t>
+  </si>
+  <si>
+    <t>NFTC-02</t>
+  </si>
+  <si>
+    <t>NFTC-03</t>
+  </si>
+  <si>
+    <t>NFTC-04</t>
+  </si>
+  <si>
+    <t>NFTC-05</t>
+  </si>
+  <si>
+    <t>NFTC-06</t>
+  </si>
+  <si>
+    <t>NFTC-07</t>
+  </si>
+  <si>
+    <t>NFTC-08</t>
+  </si>
+  <si>
+    <t>NFTC-09</t>
+  </si>
+  <si>
+    <t>NFTC-10</t>
+  </si>
+  <si>
+    <t>NFTC-11</t>
+  </si>
+  <si>
+    <t>NFTC-12</t>
+  </si>
+  <si>
+    <t>NFTC-13</t>
+  </si>
+  <si>
+    <t>NFTC-14</t>
+  </si>
+  <si>
+    <t>NFTC-15</t>
+  </si>
+  <si>
+    <t>NFTC-16</t>
+  </si>
+  <si>
+    <t>NFTC-17</t>
+  </si>
+  <si>
+    <t>NFTC-18</t>
+  </si>
+  <si>
+    <t>NFTC-19</t>
+  </si>
+  <si>
+    <t>NFTC-20</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890" }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": "fifty" }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 0.50 }</t>
+  </si>
+  <si>
+    <t>json { "username": "vikram_with_an_extra_long_username", "password": "securePass123", "email": "vikram@test.com" } "balance": -100 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 100 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "new_balance": 100 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "99999", "amount": 100 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": -50 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 0 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "67890", "amount": 100 }</t>
+  </si>
+  <si>
+    <t>json { "amount": 100 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 1000000 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "new_balance": 1000000 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 100, "currency": "INVALID" }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "67890", "amount": 100, "currency": "USD" }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists and has a balance of  150.</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists and has a balance of 50.</t>
+  </si>
+  <si>
+    <t>json { "user_id": "99999", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "67890", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>json { "amount": 50 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists and has a balance of 1000000.</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 500000 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists and has a balance of 100. Minimum withdrawal amount is 10.</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 5 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists and has a balance of 10000. Maximum withdrawal amount is 1000.</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 1500 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists and has a balance of 100.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Send a POST request to the /withdraw endpoint with an amount of 20 multiple times with different amount</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "amount": 20 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "12345", "balance": 100 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "112233", "balance": 500 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "user123", "balance": 250 }</t>
+  </si>
+  <si>
+    <t>User account with ID "45678" exists and has a high balance (e.g., 1,000,000).</t>
+  </si>
+  <si>
+    <t>json { "user_id": "45678", "balance": 1000000 }</t>
+  </si>
+  <si>
+    <t>json { "user_id": "34567", "balance": 0 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists with a balance of 100. User account with ID "67890" exists.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "new_balance": 50, "toUserId": "67890", "new_balance": 50 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists with a balance of 50. User account with ID "67890" exists.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 100 }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "99999", "toUserId": "67890", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists with a balance of 100.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "99999", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": -50 }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 0 }</t>
+  </si>
+  <si>
+    <t>Sender user account with ID "12345" exists with a balance of 100. Recipient user account with ID "67890" exists and is inactive.</t>
+  </si>
+  <si>
+    <t>json { "toUserId": "67890", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>Sender user account with ID "12345" exists with a balance of 100.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>User account with ID "12345" exists with a balance of 1,000,000. User account with ID "67890" exists.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 500000 }</t>
+  </si>
+  <si>
+    <t>```json { "fromUserId": "12345", "new_balance": 500000,</t>
+  </si>
+  <si>
+    <t>Sender user account with ID "12345" exists and is active with a balance of 100. Recipient user account with ID "67890" exists and is deactivated.</t>
+  </si>
+  <si>
+    <t>Sender user account with ID "12345" exists and is active with a balance of 100. Recipient user account with ID "67891" exists and is unverified.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67891", "amount": 50 }</t>
+  </si>
+  <si>
+    <t>User accounts with IDs "12345" and "67890" exist and are active. Maximum transfer amount is 10,000.</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 20000 }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 50, "currency": "INVALID" }</t>
+  </si>
+  <si>
+    <t>json { "fromUserId": "12345", "toUserId": "67890", "amount": 50, "currency": "USD" }</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1968,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1991,10 +2006,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2003,23 +2030,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2340,8 +2352,8 @@
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2392,52 +2404,52 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1">
-      <c r="A2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
+      <c r="A2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" s="18"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:11" ht="45">
       <c r="A4" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>385</v>
+        <v>252</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2445,25 +2457,25 @@
     </row>
     <row r="5" spans="1:11" ht="45">
       <c r="A5" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2472,25 +2484,25 @@
     </row>
     <row r="6" spans="1:11" ht="60">
       <c r="A6" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2499,25 +2511,25 @@
     </row>
     <row r="7" spans="1:11" ht="60">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>356</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>388</v>
+        <v>255</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2526,134 +2538,131 @@
     </row>
     <row r="8" spans="1:11" ht="63.75">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>357</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>389</v>
+        <v>256</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>441</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="45">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>358</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>303</v>
+        <v>190</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>304</v>
+        <v>191</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>390</v>
+        <v>257</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>309</v>
+        <v>196</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>305</v>
+        <v>192</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="45">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>359</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>306</v>
+        <v>193</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>307</v>
+        <v>194</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>391</v>
+        <v>258</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>308</v>
+        <v>195</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="A11" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" ht="45">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>360</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>392</v>
+        <v>259</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>41</v>
+        <v>442</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>42</v>
+        <v>443</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2662,25 +2671,25 @@
     </row>
     <row r="14" spans="1:11" ht="45">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>361</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>393</v>
+        <v>260</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>46</v>
+        <v>444</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2689,25 +2698,25 @@
     </row>
     <row r="15" spans="1:11" ht="45">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>362</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>394</v>
+        <v>261</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>51</v>
+        <v>445</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2716,25 +2725,25 @@
     </row>
     <row r="16" spans="1:11" ht="45">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>363</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>395</v>
+        <v>262</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>55</v>
+        <v>446</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2743,25 +2752,25 @@
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>364</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>396</v>
+        <v>263</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>61</v>
+        <v>447</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2770,25 +2779,25 @@
     </row>
     <row r="18" spans="1:11" ht="45">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>365</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>397</v>
+        <v>264</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>448</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2797,25 +2806,25 @@
     </row>
     <row r="19" spans="1:11" ht="45">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>366</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>398</v>
+        <v>265</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2824,25 +2833,25 @@
     </row>
     <row r="20" spans="1:11" ht="45">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>367</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>399</v>
+        <v>266</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2851,25 +2860,25 @@
     </row>
     <row r="21" spans="1:11" ht="45">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>368</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>400</v>
+        <v>267</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>81</v>
+        <v>449</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>82</v>
+        <v>450</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2878,105 +2887,103 @@
     </row>
     <row r="22" spans="1:11" ht="45">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>369</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>311</v>
+        <v>198</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>312</v>
+        <v>199</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>401</v>
+        <v>268</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>313</v>
+        <v>451</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>314</v>
+        <v>200</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>370</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>315</v>
+        <v>201</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>316</v>
+        <v>202</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>317</v>
+        <v>203</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>402</v>
+        <v>269</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>318</v>
+        <v>452</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>319</v>
+        <v>204</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="14"/>
+      <c r="A24" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:11" ht="45">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>371</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>125</v>
+        <v>453</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>403</v>
+        <v>270</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>87</v>
+        <v>454</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>42</v>
+        <v>443</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2985,25 +2992,25 @@
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" s="1" t="s">
-        <v>88</v>
+        <v>372</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>404</v>
+        <v>271</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>41</v>
+        <v>442</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -3012,25 +3019,25 @@
     </row>
     <row r="28" spans="1:11" ht="45">
       <c r="A28" s="1" t="s">
-        <v>93</v>
+        <v>373</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>405</v>
+        <v>272</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>96</v>
+        <v>456</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -3039,25 +3046,25 @@
     </row>
     <row r="29" spans="1:11" ht="45">
       <c r="A29" s="1" t="s">
-        <v>97</v>
+        <v>374</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>406</v>
+        <v>273</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>51</v>
+        <v>445</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -3065,25 +3072,25 @@
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" s="1" t="s">
-        <v>101</v>
+        <v>375</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>407</v>
+        <v>274</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>55</v>
+        <v>446</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -3092,25 +3099,25 @@
     </row>
     <row r="31" spans="1:11" ht="60">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>376</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>408</v>
+        <v>275</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>108</v>
+        <v>457</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -3119,25 +3126,25 @@
     </row>
     <row r="32" spans="1:11" ht="45">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>377</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>409</v>
+        <v>276</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>111</v>
+        <v>458</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -3145,25 +3152,25 @@
     </row>
     <row r="33" spans="1:11" ht="60">
       <c r="A33" s="1" t="s">
-        <v>112</v>
+        <v>378</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>410</v>
+        <v>277</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -3171,25 +3178,25 @@
     </row>
     <row r="34" spans="1:11" ht="45">
       <c r="A34" s="1" t="s">
-        <v>116</v>
+        <v>379</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>91</v>
+        <v>455</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>411</v>
+        <v>278</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -3197,25 +3204,25 @@
     </row>
     <row r="35" spans="1:11" ht="45">
       <c r="A35" s="1" t="s">
-        <v>121</v>
+        <v>380</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>123</v>
+        <v>459</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>412</v>
+        <v>279</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>124</v>
+        <v>460</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -3223,25 +3230,25 @@
     </row>
     <row r="36" spans="1:11" ht="75">
       <c r="A36" s="1" t="s">
-        <v>296</v>
+        <v>381</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>282</v>
+        <v>178</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>283</v>
+        <v>179</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>284</v>
+        <v>461</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>413</v>
+        <v>280</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>285</v>
+        <v>462</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>286</v>
+        <v>180</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -3250,25 +3257,25 @@
     </row>
     <row r="37" spans="1:11" ht="75">
       <c r="A37" s="1" t="s">
-        <v>297</v>
+        <v>382</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>287</v>
+        <v>181</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>288</v>
+        <v>182</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>289</v>
+        <v>463</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>414</v>
+        <v>281</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>290</v>
+        <v>464</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>291</v>
+        <v>183</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -3277,25 +3284,25 @@
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" s="1" t="s">
-        <v>298</v>
+        <v>383</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>292</v>
+        <v>184</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>293</v>
+        <v>185</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>294</v>
+        <v>465</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>415</v>
+        <v>466</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>295</v>
+        <v>467</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>416</v>
+        <v>282</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -3303,79 +3310,79 @@
     </row>
     <row r="39" spans="1:11" ht="60">
       <c r="A39" s="1" t="s">
-        <v>109</v>
+        <v>384</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>320</v>
+        <v>205</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>321</v>
+        <v>206</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>317</v>
+        <v>203</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>417</v>
+        <v>283</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>108</v>
+        <v>457</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>319</v>
+        <v>204</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
+      <c r="A40" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
       <c r="K40" s="12"/>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
       <c r="K41" s="12"/>
     </row>
     <row r="42" spans="1:11" ht="45">
       <c r="A42" s="1" t="s">
-        <v>128</v>
+        <v>385</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>418</v>
+        <v>284</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>132</v>
+        <v>468</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -3384,25 +3391,25 @@
     </row>
     <row r="43" spans="1:11" ht="45">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>386</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>419</v>
+        <v>285</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3411,25 +3418,25 @@
     </row>
     <row r="44" spans="1:11" ht="45">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>387</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>420</v>
+        <v>286</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -3438,52 +3445,52 @@
     </row>
     <row r="45" spans="1:11" ht="45">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>388</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>421</v>
+        <v>287</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="6"/>
       <c r="K45" s="12"/>
     </row>
-    <row r="46" spans="1:11" ht="45">
+    <row r="46" spans="1:11" ht="60">
       <c r="A46" s="1" t="s">
-        <v>141</v>
+        <v>389</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>422</v>
+        <v>288</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -3492,25 +3499,25 @@
     </row>
     <row r="47" spans="1:11" ht="45">
       <c r="A47" s="1" t="s">
-        <v>145</v>
+        <v>390</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>423</v>
+        <v>289</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>149</v>
+        <v>469</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -3518,25 +3525,25 @@
     </row>
     <row r="48" spans="1:11" ht="45">
       <c r="A48" s="1" t="s">
-        <v>150</v>
+        <v>391</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>424</v>
+        <v>290</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>154</v>
+        <v>470</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -3545,25 +3552,25 @@
     </row>
     <row r="49" spans="1:11" ht="60">
       <c r="A49" s="1" t="s">
-        <v>155</v>
+        <v>392</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>156</v>
+        <v>103</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>158</v>
+        <v>471</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>425</v>
+        <v>291</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>159</v>
+        <v>472</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -3572,25 +3579,25 @@
     </row>
     <row r="50" spans="1:11" ht="45">
       <c r="A50" s="1" t="s">
-        <v>160</v>
+        <v>393</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>426</v>
+        <v>292</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>164</v>
+        <v>473</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -3599,25 +3606,25 @@
     </row>
     <row r="51" spans="1:11" ht="60">
       <c r="A51" s="1" t="s">
-        <v>165</v>
+        <v>394</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>427</v>
+        <v>293</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -3626,25 +3633,25 @@
     </row>
     <row r="52" spans="1:11" ht="60">
       <c r="A52" s="1" t="s">
-        <v>262</v>
+        <v>395</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>263</v>
+        <v>162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>264</v>
+        <v>163</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>265</v>
+        <v>164</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>428</v>
+        <v>294</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>266</v>
+        <v>165</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -3653,25 +3660,25 @@
     </row>
     <row r="53" spans="1:11" ht="60">
       <c r="A53" s="1" t="s">
-        <v>267</v>
+        <v>396</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>268</v>
+        <v>166</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>269</v>
+        <v>167</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>270</v>
+        <v>168</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>429</v>
+        <v>295</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>271</v>
+        <v>169</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -3680,25 +3687,25 @@
     </row>
     <row r="54" spans="1:11" ht="45">
       <c r="A54" s="1" t="s">
-        <v>272</v>
+        <v>397</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>273</v>
+        <v>170</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>274</v>
+        <v>171</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>275</v>
+        <v>172</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>430</v>
+        <v>296</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>276</v>
+        <v>173</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
@@ -3707,25 +3714,25 @@
     </row>
     <row r="55" spans="1:11" ht="45">
       <c r="A55" s="1" t="s">
-        <v>277</v>
+        <v>398</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>278</v>
+        <v>174</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>279</v>
+        <v>175</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>280</v>
+        <v>176</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>431</v>
+        <v>297</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>281</v>
+        <v>177</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -3733,52 +3740,52 @@
       <c r="K55" s="12"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="14"/>
+      <c r="A56" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="17"/>
     </row>
     <row r="57" spans="1:11" ht="15" customHeight="1">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="16"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="20"/>
     </row>
     <row r="58" spans="1:11" ht="75">
       <c r="A58" s="1" t="s">
-        <v>169</v>
+        <v>399</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>170</v>
+        <v>111</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>171</v>
+        <v>112</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>172</v>
+        <v>474</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>432</v>
+        <v>298</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>173</v>
+        <v>475</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>174</v>
+        <v>476</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -3787,25 +3794,25 @@
     </row>
     <row r="59" spans="1:11" ht="75">
       <c r="A59" s="1" t="s">
-        <v>175</v>
+        <v>400</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>176</v>
+        <v>113</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>177</v>
+        <v>114</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>178</v>
+        <v>477</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>433</v>
+        <v>299</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>179</v>
+        <v>478</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -3814,25 +3821,25 @@
     </row>
     <row r="60" spans="1:11" ht="45">
       <c r="A60" s="1" t="s">
-        <v>180</v>
+        <v>401</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>434</v>
+        <v>300</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>184</v>
+        <v>479</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>185</v>
+        <v>118</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -3840,25 +3847,25 @@
     </row>
     <row r="61" spans="1:11" ht="45">
       <c r="A61" s="1" t="s">
-        <v>186</v>
+        <v>402</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>187</v>
+        <v>119</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>188</v>
+        <v>120</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>189</v>
+        <v>480</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>435</v>
+        <v>301</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>190</v>
+        <v>481</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -3866,25 +3873,25 @@
     </row>
     <row r="62" spans="1:11" ht="75">
       <c r="A62" s="1" t="s">
-        <v>192</v>
+        <v>403</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>172</v>
+        <v>474</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>436</v>
+        <v>302</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>195</v>
+        <v>482</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>196</v>
+        <v>124</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -3893,25 +3900,25 @@
     </row>
     <row r="63" spans="1:11" ht="75">
       <c r="A63" s="1" t="s">
-        <v>197</v>
+        <v>404</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>172</v>
+        <v>474</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>437</v>
+        <v>303</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>200</v>
+        <v>483</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>201</v>
+        <v>127</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -3920,25 +3927,25 @@
     </row>
     <row r="64" spans="1:11" ht="75">
       <c r="A64" s="1" t="s">
-        <v>202</v>
+        <v>405</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>203</v>
+        <v>128</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>204</v>
+        <v>129</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>205</v>
+        <v>130</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>438</v>
+        <v>304</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>173</v>
+        <v>475</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>206</v>
+        <v>131</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -3947,25 +3954,25 @@
     </row>
     <row r="65" spans="1:11" ht="90">
       <c r="A65" s="1" t="s">
-        <v>207</v>
+        <v>406</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>209</v>
+        <v>133</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>210</v>
+        <v>484</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>439</v>
+        <v>305</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>173</v>
+        <v>475</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -3974,25 +3981,25 @@
     </row>
     <row r="66" spans="1:11" ht="45">
       <c r="A66" s="1" t="s">
-        <v>212</v>
+        <v>407</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>213</v>
+        <v>135</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>214</v>
+        <v>136</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>440</v>
+        <v>306</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>215</v>
+        <v>485</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>216</v>
+        <v>137</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -4001,25 +4008,25 @@
     </row>
     <row r="67" spans="1:11" ht="60">
       <c r="A67" s="1" t="s">
-        <v>217</v>
+        <v>408</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>218</v>
+        <v>138</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>219</v>
+        <v>139</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>220</v>
+        <v>486</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>441</v>
+        <v>307</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>221</v>
+        <v>487</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>222</v>
+        <v>140</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -4028,25 +4035,25 @@
     </row>
     <row r="68" spans="1:11" ht="45">
       <c r="A68" s="1" t="s">
-        <v>223</v>
+        <v>409</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>224</v>
+        <v>141</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>225</v>
+        <v>142</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>226</v>
+        <v>143</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>442</v>
+        <v>308</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>227</v>
+        <v>438</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>228</v>
+        <v>144</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -4055,25 +4062,25 @@
     </row>
     <row r="69" spans="1:11" ht="75">
       <c r="A69" s="1" t="s">
-        <v>229</v>
+        <v>410</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>230</v>
+        <v>145</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>231</v>
+        <v>146</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>172</v>
+        <v>474</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>443</v>
+        <v>309</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>232</v>
+        <v>439</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>233</v>
+        <v>147</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -4082,25 +4089,25 @@
     </row>
     <row r="70" spans="1:11" ht="75">
       <c r="A70" s="1" t="s">
-        <v>234</v>
+        <v>411</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>235</v>
+        <v>148</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>236</v>
+        <v>149</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>237</v>
+        <v>488</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>444</v>
+        <v>310</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>238</v>
+        <v>489</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>239</v>
+        <v>490</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
@@ -4109,25 +4116,25 @@
     </row>
     <row r="71" spans="1:11" ht="105">
       <c r="A71" s="1" t="s">
-        <v>240</v>
+        <v>412</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>241</v>
+        <v>150</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>242</v>
+        <v>151</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>243</v>
+        <v>491</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>445</v>
+        <v>311</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>173</v>
+        <v>475</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>244</v>
+        <v>152</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
@@ -4136,25 +4143,25 @@
     </row>
     <row r="72" spans="1:11" ht="105">
       <c r="A72" s="1" t="s">
-        <v>245</v>
+        <v>413</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>246</v>
+        <v>153</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>247</v>
+        <v>154</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>248</v>
+        <v>492</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>446</v>
+        <v>312</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>249</v>
+        <v>493</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>250</v>
+        <v>155</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
@@ -4163,25 +4170,25 @@
     </row>
     <row r="73" spans="1:11" ht="75">
       <c r="A73" s="1" t="s">
-        <v>251</v>
+        <v>414</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>252</v>
+        <v>156</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>253</v>
+        <v>157</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>447</v>
+        <v>313</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>448</v>
+        <v>314</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>254</v>
+        <v>440</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>255</v>
+        <v>158</v>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
@@ -4189,53 +4196,53 @@
       <c r="K73" s="12"/>
     </row>
     <row r="74" spans="1:11" ht="75">
-      <c r="A74" s="3" t="s">
-        <v>256</v>
+      <c r="A74" s="1" t="s">
+        <v>415</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>257</v>
+        <v>159</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>258</v>
+        <v>160</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>259</v>
+        <v>494</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>449</v>
+        <v>315</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>260</v>
+        <v>495</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>261</v>
+        <v>161</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
-      <c r="J74" s="21"/>
+      <c r="J74" s="13"/>
       <c r="K74" s="12"/>
     </row>
     <row r="75" spans="1:11" ht="90">
       <c r="A75" s="1" t="s">
-        <v>322</v>
+        <v>416</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>323</v>
+        <v>207</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>324</v>
+        <v>208</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>325</v>
+        <v>209</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>450</v>
+        <v>316</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>326</v>
+        <v>496</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>314</v>
+        <v>200</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
@@ -4243,578 +4250,578 @@
     </row>
     <row r="76" spans="1:11" ht="105">
       <c r="A76" s="1" t="s">
-        <v>327</v>
+        <v>417</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>328</v>
+        <v>210</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>329</v>
+        <v>211</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>330</v>
+        <v>212</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>451</v>
+        <v>317</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>331</v>
+        <v>497</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>332</v>
+        <v>213</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="14"/>
+      <c r="A77" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="17"/>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="15"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="15"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="16"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="20"/>
     </row>
     <row r="79" spans="1:11" ht="75">
       <c r="A79" s="1" t="s">
-        <v>344</v>
+        <v>418</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>345</v>
+        <v>222</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>347</v>
+        <v>224</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>489</v>
+        <v>349</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="H79" s="22"/>
-      <c r="I79" s="22"/>
+        <v>223</v>
+      </c>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
       <c r="J79" s="1"/>
     </row>
     <row r="80" spans="1:11" ht="60">
       <c r="A80" s="1" t="s">
-        <v>486</v>
+        <v>419</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>336</v>
+        <v>216</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>350</v>
+        <v>226</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>452</v>
+        <v>318</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
+        <v>217</v>
+      </c>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
       <c r="J80" s="1"/>
     </row>
     <row r="81" spans="1:10" ht="75">
       <c r="A81" s="1" t="s">
-        <v>487</v>
+        <v>420</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>339</v>
+        <v>218</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>351</v>
+        <v>227</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>453</v>
+        <v>319</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="H81" s="22"/>
-      <c r="I81" s="22"/>
+        <v>219</v>
+      </c>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
       <c r="J81" s="1"/>
     </row>
     <row r="82" spans="1:10" ht="90">
       <c r="A82" s="1" t="s">
-        <v>488</v>
+        <v>421</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>342</v>
+        <v>220</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>352</v>
+        <v>228</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>334</v>
+        <v>215</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>454</v>
+        <v>320</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="H82" s="22"/>
-      <c r="I82" s="22"/>
+        <v>221</v>
+      </c>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
       <c r="J82" s="1"/>
     </row>
     <row r="83" spans="1:10" ht="60">
       <c r="A83" s="1" t="s">
-        <v>468</v>
+        <v>422</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>354</v>
+        <v>229</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>349</v>
+        <v>225</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>355</v>
+        <v>230</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>455</v>
+        <v>321</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="H83" s="22"/>
-      <c r="I83" s="22"/>
+        <v>231</v>
+      </c>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
       <c r="J83" s="1"/>
     </row>
     <row r="84" spans="1:10" ht="45">
       <c r="A84" s="1" t="s">
-        <v>474</v>
+        <v>423</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>358</v>
+        <v>232</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>350</v>
+        <v>226</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>355</v>
+        <v>230</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>456</v>
+        <v>322</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H84" s="22"/>
-      <c r="I84" s="22"/>
+        <v>217</v>
+      </c>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
       <c r="J84" s="1"/>
     </row>
     <row r="85" spans="1:10" ht="75">
       <c r="A85" s="1" t="s">
-        <v>480</v>
+        <v>424</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>360</v>
+        <v>233</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>351</v>
+        <v>227</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>355</v>
+        <v>230</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>453</v>
+        <v>319</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H85" s="22"/>
-      <c r="I85" s="22"/>
+        <v>234</v>
+      </c>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="1:10" ht="60">
       <c r="A86" s="1" t="s">
-        <v>348</v>
+        <v>425</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>363</v>
+        <v>235</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>349</v>
+        <v>225</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>364</v>
+        <v>236</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>457</v>
+        <v>323</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>465</v>
+        <v>331</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="H86" s="22"/>
-      <c r="I86" s="22"/>
+        <v>231</v>
+      </c>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="1:10" ht="45">
       <c r="A87" s="1" t="s">
-        <v>335</v>
+        <v>426</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>366</v>
+        <v>237</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>350</v>
+        <v>226</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>364</v>
+        <v>236</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>458</v>
+        <v>324</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>465</v>
+        <v>331</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H87" s="22"/>
-      <c r="I87" s="22"/>
+        <v>217</v>
+      </c>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="1:10" ht="75">
       <c r="A88" s="1" t="s">
-        <v>338</v>
+        <v>427</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>368</v>
+        <v>238</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>351</v>
+        <v>227</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>364</v>
+        <v>236</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>453</v>
+        <v>319</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>465</v>
+        <v>331</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H88" s="22"/>
-      <c r="I88" s="22"/>
+        <v>234</v>
+      </c>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="1:10" ht="60">
       <c r="A89" s="1" t="s">
-        <v>341</v>
+        <v>428</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>370</v>
+        <v>239</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>349</v>
+        <v>225</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>371</v>
+        <v>240</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>459</v>
+        <v>325</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>466</v>
+        <v>332</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="H89" s="22"/>
-      <c r="I89" s="22"/>
+        <v>231</v>
+      </c>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="1:10" ht="60">
       <c r="A90" s="1" t="s">
-        <v>353</v>
+        <v>429</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>373</v>
+        <v>241</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>350</v>
+        <v>226</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>371</v>
+        <v>240</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>460</v>
+        <v>326</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>466</v>
+        <v>332</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H90" s="22"/>
-      <c r="I90" s="22"/>
+        <v>217</v>
+      </c>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="1:10" ht="75">
       <c r="A91" s="1" t="s">
-        <v>357</v>
+        <v>430</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>375</v>
+        <v>242</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>351</v>
+        <v>227</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>371</v>
+        <v>240</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>453</v>
+        <v>319</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>466</v>
+        <v>332</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H91" s="22"/>
-      <c r="I91" s="22"/>
+        <v>234</v>
+      </c>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="1:10" ht="60">
       <c r="A92" s="1" t="s">
-        <v>359</v>
+        <v>431</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>376</v>
+        <v>243</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>349</v>
+        <v>225</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>377</v>
+        <v>244</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>461</v>
+        <v>327</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>467</v>
+        <v>333</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="H92" s="22"/>
-      <c r="I92" s="22"/>
+        <v>231</v>
+      </c>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="1:10" ht="45">
       <c r="A93" s="1" t="s">
-        <v>362</v>
+        <v>432</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>378</v>
+        <v>245</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>350</v>
+        <v>226</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>377</v>
+        <v>244</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>462</v>
+        <v>328</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>467</v>
+        <v>333</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H93" s="22"/>
-      <c r="I93" s="22"/>
+        <v>217</v>
+      </c>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="1:10" ht="105">
       <c r="A94" s="1" t="s">
-        <v>365</v>
+        <v>433</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>379</v>
+        <v>246</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>381</v>
+        <v>248</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>377</v>
+        <v>244</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>463</v>
+        <v>329</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>467</v>
+        <v>333</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
+        <v>247</v>
+      </c>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="1:10" ht="75">
       <c r="A95" s="1" t="s">
-        <v>367</v>
+        <v>434</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>382</v>
+        <v>249</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>384</v>
+        <v>251</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>377</v>
+        <v>244</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>464</v>
+        <v>330</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>467</v>
+        <v>333</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
-      <c r="J95" s="22"/>
-    </row>
-    <row r="96" spans="1:10" ht="105">
+        <v>250</v>
+      </c>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+    </row>
+    <row r="96" spans="1:10" ht="90">
       <c r="A96" s="1" t="s">
-        <v>369</v>
+        <v>435</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>469</v>
+        <v>334</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>470</v>
+        <v>335</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>471</v>
+        <v>336</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>490</v>
+        <v>350</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>472</v>
+        <v>337</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="H96" s="22"/>
-      <c r="I96" s="22"/>
-      <c r="J96" s="22"/>
+        <v>338</v>
+      </c>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
     </row>
     <row r="97" spans="1:10" ht="60">
       <c r="A97" s="1" t="s">
-        <v>372</v>
+        <v>436</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>475</v>
+        <v>339</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>476</v>
+        <v>340</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>477</v>
+        <v>341</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>491</v>
+        <v>351</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>478</v>
+        <v>342</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="H97" s="22"/>
-      <c r="I97" s="22"/>
-      <c r="J97" s="22"/>
-    </row>
-    <row r="98" spans="1:10" ht="90">
+        <v>343</v>
+      </c>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="1:10" ht="75">
       <c r="A98" s="1" t="s">
-        <v>374</v>
+        <v>437</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>481</v>
+        <v>344</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>482</v>
+        <v>345</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>483</v>
+        <v>346</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>492</v>
+        <v>352</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>484</v>
+        <v>347</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="H98" s="22"/>
-      <c r="I98" s="22"/>
-      <c r="J98" s="22"/>
+        <v>348</v>
+      </c>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:J3"/>
     <mergeCell ref="A77:J78"/>
     <mergeCell ref="A56:J57"/>
     <mergeCell ref="A40:J41"/>
     <mergeCell ref="A24:J25"/>
     <mergeCell ref="A11:J12"/>
-    <mergeCell ref="A2:J3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>